<commit_message>
Rename isLDS to isLDES, adjust unit of demand (to MW)
</commit_message>
<xml_diff>
--- a/data/example/Power_Demand.xlsx
+++ b/data/example/Power_Demand.xlsx
@@ -665,7 +665,7 @@
       </c>
       <c r="C2" s="4" t="inlineStr">
         <is>
-          <t>v0.1.2</t>
+          <t>v0.1.3</t>
         </is>
       </c>
     </row>
@@ -1193,122 +1193,122 @@
       </c>
       <c r="G7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="H7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="I7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="J7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="K7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="L7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="M7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="N7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="O7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="P7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="Q7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="R7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="S7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="T7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="U7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="V7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="W7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="X7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="Y7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="Z7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="AA7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="AB7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="AC7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="AD7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
     </row>
@@ -7523,7 +7523,7 @@
       </c>
       <c r="C2" s="4" t="inlineStr">
         <is>
-          <t>v0.1.2</t>
+          <t>v0.1.3</t>
         </is>
       </c>
     </row>
@@ -8051,122 +8051,122 @@
       </c>
       <c r="G7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="H7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="I7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="J7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="K7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="L7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="M7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="N7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="O7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="P7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="Q7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="R7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="S7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="T7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="U7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="V7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="W7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="X7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="Y7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="Z7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="AA7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="AB7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="AC7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
       <c r="AD7" s="10" t="inlineStr">
         <is>
-          <t>[MWh]</t>
+          <t>[MW]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Adjust description of Power_Demand (-> v0.1.4)
</commit_message>
<xml_diff>
--- a/data/example/Power_Demand.xlsx
+++ b/data/example/Power_Demand.xlsx
@@ -572,7 +572,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <tabColor rgb="00008080"/>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -665,7 +665,7 @@
       </c>
       <c r="C2" s="4" t="inlineStr">
         <is>
-          <t>v0.1.3</t>
+          <t>v0.1.4</t>
         </is>
       </c>
     </row>
@@ -991,7 +991,7 @@
       </c>
       <c r="G5" s="8" t="inlineStr">
         <is>
-          <t>Demand at node for representative hour k</t>
+          <t>Demand at this representative time step k</t>
         </is>
       </c>
       <c r="H5" s="7" t="n"/>
@@ -7425,12 +7425,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <legacyDrawing r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <tabColor rgb="00008080"/>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -7523,7 +7523,7 @@
       </c>
       <c r="C2" s="4" t="inlineStr">
         <is>
-          <t>v0.1.3</t>
+          <t>v0.1.4</t>
         </is>
       </c>
     </row>
@@ -7849,7 +7849,7 @@
       </c>
       <c r="G5" s="8" t="inlineStr">
         <is>
-          <t>Demand at node for representative hour k</t>
+          <t>Demand at this representative time step k</t>
         </is>
       </c>
       <c r="H5" s="7" t="n"/>
@@ -14283,6 +14283,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <legacyDrawing r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
</xml_diff>